<commit_message>
Fixed TAC Template excel sheet
</commit_message>
<xml_diff>
--- a/TAC_Template.xlsx
+++ b/TAC_Template.xlsx
@@ -1,23 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27907"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28016"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Research_Macbook/Desktop/Excel_Sheets/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Research_Macbook/GitHub/Excel_Files/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="640" yWindow="460" windowWidth="24960" windowHeight="13920" tabRatio="500"/>
+    <workbookView xWindow="2220" yWindow="1160" windowWidth="24960" windowHeight="13920" tabRatio="500"/>
   </bookViews>
   <sheets>
-    <sheet name="Image Derived Input Function" sheetId="2" r:id="rId1"/>
+    <sheet name="TAC" sheetId="2" r:id="rId1"/>
     <sheet name="Sheet1" sheetId="1" r:id="rId2"/>
   </sheets>
-  <externalReferences>
-    <externalReference r:id="rId3"/>
-  </externalReferences>
   <calcPr calcId="150000" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
@@ -31,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t>Time [seconds]</t>
   </si>
@@ -64,6 +61,12 @@
   </si>
   <si>
     <t>Date</t>
+  </si>
+  <si>
+    <t>Tracer</t>
+  </si>
+  <si>
+    <t>Patient ID</t>
   </si>
 </sst>
 </file>
@@ -237,12 +240,9 @@
     <xf numFmtId="0" fontId="6" fillId="2" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="3" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="4"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="5"/>
     <xf numFmtId="2" fontId="6" fillId="2" borderId="3" xfId="6" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -256,13 +256,14 @@
     <xf numFmtId="2" fontId="4" fillId="3" borderId="4" xfId="3" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyAlignment="1"/>
     <xf numFmtId="19" fontId="8" fillId="2" borderId="5" xfId="6" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="2"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1"/>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="3" xfId="6"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="8">
@@ -374,7 +375,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Image Derived Input Function'!$B$4</c:f>
+              <c:f>TAC!$B$4</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -409,7 +410,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>'Image Derived Input Function'!$A$5:$A$62</c:f>
+              <c:f>TAC!$A$5:$A$62</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="58"/>
@@ -418,7 +419,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'Image Derived Input Function'!$B$5:$B$62</c:f>
+              <c:f>TAC!$B$5:$B$62</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="58"/>
@@ -435,11 +436,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-1900689280"/>
-        <c:axId val="-1900686160"/>
+        <c:axId val="1945170704"/>
+        <c:axId val="1981014000"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-1900689280"/>
+        <c:axId val="1945170704"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -557,12 +558,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1900686160"/>
+        <c:crossAx val="1981014000"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-1900686160"/>
+        <c:axId val="1981014000"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -679,7 +680,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1900689280"/>
+        <c:crossAx val="1945170704"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -817,7 +818,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Image Derived Input Function'!$C$4</c:f>
+              <c:f>TAC!$C$4</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -852,7 +853,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>'Image Derived Input Function'!$A$5:$A$62</c:f>
+              <c:f>TAC!$A$5:$A$62</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="58"/>
@@ -861,7 +862,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'Image Derived Input Function'!$C$5:$C$62</c:f>
+              <c:f>TAC!$C$5:$C$62</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="58"/>
@@ -1052,11 +1053,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-1900652272"/>
-        <c:axId val="-1900649152"/>
+        <c:axId val="1835020464"/>
+        <c:axId val="1907509552"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-1900652272"/>
+        <c:axId val="1835020464"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1169,12 +1170,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1900649152"/>
+        <c:crossAx val="1907509552"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-1900649152"/>
+        <c:axId val="1907509552"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1286,7 +1287,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1900652272"/>
+        <c:crossAx val="1835020464"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2451,16 +2452,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>31750</xdr:colOff>
-      <xdr:row>3</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>44450</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>25400</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>812800</xdr:colOff>
-      <xdr:row>30</xdr:row>
-      <xdr:rowOff>88900</xdr:rowOff>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>393700</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>139700</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2514,332 +2515,6 @@
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
-</file>
-
-<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
-  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
-    <sheetNames>
-      <sheetName val="Input Function Calculation"/>
-      <sheetName val="Plot"/>
-      <sheetName val="Extra Info"/>
-      <sheetName val="Image Derived Input Function"/>
-      <sheetName val="RAW"/>
-    </sheetNames>
-    <sheetDataSet>
-      <sheetData sheetId="0">
-        <row r="10">
-          <cell r="E10">
-            <v>0</v>
-          </cell>
-        </row>
-      </sheetData>
-      <sheetData sheetId="1" refreshError="1"/>
-      <sheetData sheetId="2" refreshError="1"/>
-      <sheetData sheetId="3">
-        <row r="1">
-          <cell r="B1" t="str">
-            <v>Averaged [kBq/cc]</v>
-          </cell>
-          <cell r="C1" t="str">
-            <v>% of Injected Dose</v>
-          </cell>
-        </row>
-        <row r="2">
-          <cell r="C2" t="e">
-            <v>#DIV/0!</v>
-          </cell>
-        </row>
-        <row r="3">
-          <cell r="C3" t="e">
-            <v>#DIV/0!</v>
-          </cell>
-        </row>
-        <row r="4">
-          <cell r="C4" t="e">
-            <v>#DIV/0!</v>
-          </cell>
-        </row>
-        <row r="5">
-          <cell r="C5" t="e">
-            <v>#DIV/0!</v>
-          </cell>
-        </row>
-        <row r="6">
-          <cell r="C6" t="e">
-            <v>#DIV/0!</v>
-          </cell>
-        </row>
-        <row r="7">
-          <cell r="C7" t="e">
-            <v>#DIV/0!</v>
-          </cell>
-        </row>
-        <row r="8">
-          <cell r="C8" t="e">
-            <v>#DIV/0!</v>
-          </cell>
-        </row>
-        <row r="9">
-          <cell r="C9" t="e">
-            <v>#DIV/0!</v>
-          </cell>
-        </row>
-        <row r="10">
-          <cell r="C10" t="e">
-            <v>#DIV/0!</v>
-          </cell>
-        </row>
-        <row r="11">
-          <cell r="C11" t="e">
-            <v>#DIV/0!</v>
-          </cell>
-        </row>
-        <row r="12">
-          <cell r="C12" t="e">
-            <v>#DIV/0!</v>
-          </cell>
-        </row>
-        <row r="13">
-          <cell r="C13" t="e">
-            <v>#DIV/0!</v>
-          </cell>
-        </row>
-        <row r="14">
-          <cell r="C14" t="e">
-            <v>#DIV/0!</v>
-          </cell>
-        </row>
-        <row r="15">
-          <cell r="C15" t="e">
-            <v>#DIV/0!</v>
-          </cell>
-        </row>
-        <row r="16">
-          <cell r="C16" t="e">
-            <v>#DIV/0!</v>
-          </cell>
-        </row>
-        <row r="17">
-          <cell r="C17" t="e">
-            <v>#DIV/0!</v>
-          </cell>
-        </row>
-        <row r="18">
-          <cell r="C18" t="e">
-            <v>#DIV/0!</v>
-          </cell>
-        </row>
-        <row r="19">
-          <cell r="C19" t="e">
-            <v>#DIV/0!</v>
-          </cell>
-        </row>
-        <row r="20">
-          <cell r="C20" t="e">
-            <v>#DIV/0!</v>
-          </cell>
-        </row>
-        <row r="21">
-          <cell r="C21" t="e">
-            <v>#DIV/0!</v>
-          </cell>
-        </row>
-        <row r="22">
-          <cell r="C22" t="e">
-            <v>#DIV/0!</v>
-          </cell>
-        </row>
-        <row r="23">
-          <cell r="C23" t="e">
-            <v>#DIV/0!</v>
-          </cell>
-        </row>
-        <row r="24">
-          <cell r="C24" t="e">
-            <v>#DIV/0!</v>
-          </cell>
-        </row>
-        <row r="25">
-          <cell r="C25" t="e">
-            <v>#DIV/0!</v>
-          </cell>
-        </row>
-        <row r="26">
-          <cell r="C26" t="e">
-            <v>#DIV/0!</v>
-          </cell>
-        </row>
-        <row r="27">
-          <cell r="C27" t="e">
-            <v>#DIV/0!</v>
-          </cell>
-        </row>
-        <row r="28">
-          <cell r="C28" t="e">
-            <v>#DIV/0!</v>
-          </cell>
-        </row>
-        <row r="29">
-          <cell r="C29" t="e">
-            <v>#DIV/0!</v>
-          </cell>
-        </row>
-        <row r="30">
-          <cell r="C30" t="e">
-            <v>#DIV/0!</v>
-          </cell>
-        </row>
-        <row r="31">
-          <cell r="C31" t="e">
-            <v>#DIV/0!</v>
-          </cell>
-        </row>
-        <row r="32">
-          <cell r="C32" t="e">
-            <v>#DIV/0!</v>
-          </cell>
-        </row>
-        <row r="33">
-          <cell r="C33" t="e">
-            <v>#DIV/0!</v>
-          </cell>
-        </row>
-        <row r="34">
-          <cell r="C34" t="e">
-            <v>#DIV/0!</v>
-          </cell>
-        </row>
-        <row r="35">
-          <cell r="C35" t="e">
-            <v>#DIV/0!</v>
-          </cell>
-        </row>
-        <row r="36">
-          <cell r="C36" t="e">
-            <v>#DIV/0!</v>
-          </cell>
-        </row>
-        <row r="37">
-          <cell r="C37" t="e">
-            <v>#DIV/0!</v>
-          </cell>
-        </row>
-        <row r="38">
-          <cell r="C38" t="e">
-            <v>#DIV/0!</v>
-          </cell>
-        </row>
-        <row r="39">
-          <cell r="C39" t="e">
-            <v>#DIV/0!</v>
-          </cell>
-        </row>
-        <row r="40">
-          <cell r="C40" t="e">
-            <v>#DIV/0!</v>
-          </cell>
-        </row>
-        <row r="41">
-          <cell r="C41" t="e">
-            <v>#DIV/0!</v>
-          </cell>
-        </row>
-        <row r="42">
-          <cell r="C42" t="e">
-            <v>#DIV/0!</v>
-          </cell>
-        </row>
-        <row r="43">
-          <cell r="C43" t="e">
-            <v>#DIV/0!</v>
-          </cell>
-        </row>
-        <row r="44">
-          <cell r="C44" t="e">
-            <v>#DIV/0!</v>
-          </cell>
-        </row>
-        <row r="45">
-          <cell r="C45" t="e">
-            <v>#DIV/0!</v>
-          </cell>
-        </row>
-        <row r="46">
-          <cell r="C46" t="e">
-            <v>#DIV/0!</v>
-          </cell>
-        </row>
-        <row r="47">
-          <cell r="C47" t="e">
-            <v>#DIV/0!</v>
-          </cell>
-        </row>
-        <row r="48">
-          <cell r="C48" t="e">
-            <v>#DIV/0!</v>
-          </cell>
-        </row>
-        <row r="49">
-          <cell r="C49" t="e">
-            <v>#DIV/0!</v>
-          </cell>
-        </row>
-        <row r="50">
-          <cell r="C50" t="e">
-            <v>#DIV/0!</v>
-          </cell>
-        </row>
-        <row r="51">
-          <cell r="C51" t="e">
-            <v>#DIV/0!</v>
-          </cell>
-        </row>
-        <row r="52">
-          <cell r="C52" t="e">
-            <v>#DIV/0!</v>
-          </cell>
-        </row>
-        <row r="53">
-          <cell r="C53" t="e">
-            <v>#DIV/0!</v>
-          </cell>
-        </row>
-        <row r="54">
-          <cell r="C54" t="e">
-            <v>#DIV/0!</v>
-          </cell>
-        </row>
-        <row r="55">
-          <cell r="C55" t="e">
-            <v>#DIV/0!</v>
-          </cell>
-        </row>
-        <row r="56">
-          <cell r="C56" t="e">
-            <v>#DIV/0!</v>
-          </cell>
-        </row>
-        <row r="57">
-          <cell r="C57" t="e">
-            <v>#DIV/0!</v>
-          </cell>
-        </row>
-        <row r="58">
-          <cell r="C58" t="e">
-            <v>#DIV/0!</v>
-          </cell>
-        </row>
-        <row r="59">
-          <cell r="C59" t="e">
-            <v>#DIV/0!</v>
-          </cell>
-        </row>
-      </sheetData>
-      <sheetData sheetId="4" refreshError="1"/>
-    </sheetDataSet>
-  </externalBook>
-</externalLink>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -3106,51 +2781,59 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet3" enableFormatConditionsCalculation="0"/>
-  <dimension ref="A1:E62"/>
+  <dimension ref="A1:G62"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="D20" sqref="D20"/>
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="17.33203125" style="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.6640625" style="3" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.5" style="3" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.6640625" style="3" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16" style="3" bestFit="1" customWidth="1"/>
-    <col min="6" max="16384" width="10.83203125" style="3"/>
+    <col min="1" max="1" width="17.33203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.6640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.83203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.1640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18.5" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.6640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16" style="2" bestFit="1" customWidth="1"/>
+    <col min="8" max="16384" width="10.83203125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="21" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="8" t="s">
+    <row r="1" spans="1:7" ht="21" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="B1" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="B1" s="13" t="s">
+      <c r="C1" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="C1" s="11" t="s">
+      <c r="D1" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="E1" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="D1" s="11" t="s">
+      <c r="F1" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="E1" s="11" t="s">
+      <c r="G1" s="10" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="22" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="9">
+    <row r="2" spans="1:7" ht="22" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="7"/>
+      <c r="B2" s="7">
         <v>0.5</v>
       </c>
-      <c r="B2" s="12"/>
-      <c r="C2" s="10">
-        <v>10</v>
-      </c>
-      <c r="D2" s="10"/>
-      <c r="E2" s="10"/>
-    </row>
-    <row r="4" spans="1:5" ht="21" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C2" s="9"/>
+      <c r="D2" s="9"/>
+      <c r="E2" s="8"/>
+      <c r="F2" s="8"/>
+      <c r="G2" s="8"/>
+    </row>
+    <row r="4" spans="1:7" ht="21" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>0</v>
       </c>
@@ -3160,17 +2843,17 @@
       <c r="C4" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D4" s="2" t="s">
+      <c r="D4" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="E4" s="2"/>
-    </row>
-    <row r="5" spans="1:5" ht="19" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="4"/>
-      <c r="B5" s="4"/>
-      <c r="C5" s="5">
-        <f>B5/(C2*37000)</f>
-        <v>0</v>
+      <c r="E4" s="11"/>
+    </row>
+    <row r="5" spans="1:7" ht="19" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="3"/>
+      <c r="B5" s="3"/>
+      <c r="C5" s="4" t="e">
+        <f>B5/(E2*37000)</f>
+        <v>#DIV/0!</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>4</v>
@@ -3179,468 +2862,468 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="17" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="4"/>
-      <c r="B6" s="4"/>
-      <c r="C6" s="5">
-        <f>B6/(C2*37000)</f>
-        <v>0</v>
-      </c>
-      <c r="D6" s="6" t="e">
+    <row r="6" spans="1:7" ht="17" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="3"/>
+      <c r="B6" s="3"/>
+      <c r="C6" s="4" t="e">
+        <f>B6/(E2*37000)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="D6" s="5" t="e">
         <f>INDEX($A$4:$A$62,MATCH(MAX($B$4:$B$62),$B$4:$B$62,0))</f>
         <v>#N/A</v>
       </c>
-      <c r="E6" s="7">
+      <c r="E6" s="6">
         <f>MAX(B5:B62)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A7" s="4"/>
-      <c r="B7" s="4"/>
-      <c r="C7" s="5">
-        <f>B7/(C2*37000)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A8" s="4"/>
-      <c r="B8" s="4"/>
-      <c r="C8" s="5">
-        <f>B8/(C2*37000)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A9" s="4"/>
-      <c r="B9" s="4"/>
-      <c r="C9" s="5">
-        <f>B9/(C2*37000)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A10" s="4"/>
-      <c r="B10" s="4"/>
-      <c r="C10" s="5">
-        <f>B10/(C2*37000)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A11" s="4"/>
-      <c r="B11" s="4"/>
-      <c r="C11" s="5">
-        <f>B11/(C2*37000)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A12" s="4"/>
-      <c r="B12" s="4"/>
-      <c r="C12" s="5">
-        <f>B12/(C2*37000)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A13" s="4"/>
-      <c r="B13" s="4"/>
-      <c r="C13" s="5">
-        <f>B13/(C2*37000)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A14" s="4"/>
-      <c r="B14" s="4"/>
-      <c r="C14" s="5">
-        <f>B14/(C2*37000)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A15" s="4"/>
-      <c r="B15" s="4"/>
-      <c r="C15" s="5">
-        <f>B15/(C2*37000)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A16" s="4"/>
-      <c r="B16" s="4"/>
-      <c r="C16" s="5">
-        <f>B16/(C2*37000)</f>
-        <v>0</v>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A7" s="3"/>
+      <c r="B7" s="3"/>
+      <c r="C7" s="4" t="e">
+        <f>B7/(E2*37000)</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A8" s="3"/>
+      <c r="B8" s="3"/>
+      <c r="C8" s="4" t="e">
+        <f>B8/(E2*37000)</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A9" s="3"/>
+      <c r="B9" s="3"/>
+      <c r="C9" s="4" t="e">
+        <f>B9/(E2*37000)</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A10" s="3"/>
+      <c r="B10" s="3"/>
+      <c r="C10" s="4" t="e">
+        <f>B10/(E2*37000)</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A11" s="3"/>
+      <c r="B11" s="3"/>
+      <c r="C11" s="4" t="e">
+        <f>B11/(E2*37000)</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A12" s="3"/>
+      <c r="B12" s="3"/>
+      <c r="C12" s="4" t="e">
+        <f>B12/(E2*37000)</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A13" s="3"/>
+      <c r="B13" s="3"/>
+      <c r="C13" s="4" t="e">
+        <f>B13/(E2*37000)</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A14" s="3"/>
+      <c r="B14" s="3"/>
+      <c r="C14" s="4" t="e">
+        <f>B14/(E2*37000)</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A15" s="3"/>
+      <c r="B15" s="3"/>
+      <c r="C15" s="4" t="e">
+        <f>B15/(E2*37000)</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A16" s="3"/>
+      <c r="B16" s="3"/>
+      <c r="C16" s="4" t="e">
+        <f>B16/(E2*37000)</f>
+        <v>#DIV/0!</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A17" s="4"/>
-      <c r="B17" s="4"/>
-      <c r="C17" s="5">
-        <f>B17/(C2*37000)</f>
-        <v>0</v>
+      <c r="A17" s="3"/>
+      <c r="B17" s="3"/>
+      <c r="C17" s="4" t="e">
+        <f>B17/(E2*37000)</f>
+        <v>#DIV/0!</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A18" s="4"/>
-      <c r="B18" s="4"/>
-      <c r="C18" s="5">
-        <f>B18/(C2*37000)</f>
-        <v>0</v>
+      <c r="A18" s="3"/>
+      <c r="B18" s="3"/>
+      <c r="C18" s="4" t="e">
+        <f>B18/(E2*37000)</f>
+        <v>#DIV/0!</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A19" s="4"/>
-      <c r="B19" s="4"/>
-      <c r="C19" s="5">
-        <f>B19/(C2*37000)</f>
-        <v>0</v>
+      <c r="A19" s="3"/>
+      <c r="B19" s="3"/>
+      <c r="C19" s="4" t="e">
+        <f>B19/(E2*37000)</f>
+        <v>#DIV/0!</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A20" s="4"/>
-      <c r="B20" s="4"/>
-      <c r="C20" s="5">
-        <f>B20/(C2*37000)</f>
-        <v>0</v>
+      <c r="A20" s="3"/>
+      <c r="B20" s="3"/>
+      <c r="C20" s="4" t="e">
+        <f>B20/(E2*37000)</f>
+        <v>#DIV/0!</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A21" s="4"/>
-      <c r="B21" s="4"/>
-      <c r="C21" s="5">
-        <f>B21/(C2*37000)</f>
-        <v>0</v>
+      <c r="A21" s="3"/>
+      <c r="B21" s="3"/>
+      <c r="C21" s="4" t="e">
+        <f>B21/(E2*37000)</f>
+        <v>#DIV/0!</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A22" s="4"/>
-      <c r="B22" s="4"/>
-      <c r="C22" s="5">
-        <f>B22/(C2*37000)</f>
-        <v>0</v>
+      <c r="A22" s="3"/>
+      <c r="B22" s="3"/>
+      <c r="C22" s="4" t="e">
+        <f>B22/(E2*37000)</f>
+        <v>#DIV/0!</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A23" s="4"/>
-      <c r="B23" s="4"/>
-      <c r="C23" s="5">
-        <f>B23/(C2*37000)</f>
-        <v>0</v>
+      <c r="A23" s="3"/>
+      <c r="B23" s="3"/>
+      <c r="C23" s="4" t="e">
+        <f>B23/(E2*37000)</f>
+        <v>#DIV/0!</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A24" s="4"/>
-      <c r="B24" s="4"/>
-      <c r="C24" s="5">
-        <f>B24/(C2*37000)</f>
-        <v>0</v>
+      <c r="A24" s="3"/>
+      <c r="B24" s="3"/>
+      <c r="C24" s="4" t="e">
+        <f>B24/(E2*37000)</f>
+        <v>#DIV/0!</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A25" s="4"/>
-      <c r="B25" s="4"/>
-      <c r="C25" s="5">
-        <f>B25/(C2*37000)</f>
-        <v>0</v>
+      <c r="A25" s="3"/>
+      <c r="B25" s="3"/>
+      <c r="C25" s="4" t="e">
+        <f>B25/(E2*37000)</f>
+        <v>#DIV/0!</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A26" s="4"/>
-      <c r="B26" s="4"/>
-      <c r="C26" s="5">
-        <f>B26/(C2*37000)</f>
-        <v>0</v>
+      <c r="A26" s="3"/>
+      <c r="B26" s="3"/>
+      <c r="C26" s="4" t="e">
+        <f>B26/(E2*37000)</f>
+        <v>#DIV/0!</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A27" s="4"/>
-      <c r="B27" s="4"/>
-      <c r="C27" s="5">
-        <f>B27/(C2*37000)</f>
-        <v>0</v>
+      <c r="A27" s="3"/>
+      <c r="B27" s="3"/>
+      <c r="C27" s="4" t="e">
+        <f>B27/(E2*37000)</f>
+        <v>#DIV/0!</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A28" s="4"/>
-      <c r="B28" s="4"/>
-      <c r="C28" s="5">
-        <f>B28/(C2*37000)</f>
-        <v>0</v>
+      <c r="A28" s="3"/>
+      <c r="B28" s="3"/>
+      <c r="C28" s="4" t="e">
+        <f>B28/(E2*37000)</f>
+        <v>#DIV/0!</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A29" s="4"/>
-      <c r="B29" s="4"/>
-      <c r="C29" s="5">
-        <f>B29/(C2*37000)</f>
-        <v>0</v>
+      <c r="A29" s="3"/>
+      <c r="B29" s="3"/>
+      <c r="C29" s="4" t="e">
+        <f>B29/(E2*37000)</f>
+        <v>#DIV/0!</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A30" s="4"/>
-      <c r="B30" s="4"/>
-      <c r="C30" s="5">
-        <f>B30/(C2*37000)</f>
-        <v>0</v>
+      <c r="A30" s="3"/>
+      <c r="B30" s="3"/>
+      <c r="C30" s="4" t="e">
+        <f>B30/(E2*37000)</f>
+        <v>#DIV/0!</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A31" s="4"/>
-      <c r="B31" s="4"/>
-      <c r="C31" s="5">
-        <f>B31/(C2*37000)</f>
-        <v>0</v>
+      <c r="A31" s="3"/>
+      <c r="B31" s="3"/>
+      <c r="C31" s="4" t="e">
+        <f>B31/(E2*37000)</f>
+        <v>#DIV/0!</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A32" s="4"/>
-      <c r="B32" s="4"/>
-      <c r="C32" s="5">
-        <f>B32/(C2*37000)</f>
-        <v>0</v>
+      <c r="A32" s="3"/>
+      <c r="B32" s="3"/>
+      <c r="C32" s="4" t="e">
+        <f>B32/(E2*37000)</f>
+        <v>#DIV/0!</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A33" s="4"/>
-      <c r="B33" s="4"/>
-      <c r="C33" s="5">
-        <f>B33/(C2*37000)</f>
-        <v>0</v>
+      <c r="A33" s="3"/>
+      <c r="B33" s="3"/>
+      <c r="C33" s="4" t="e">
+        <f>B33/(E2*37000)</f>
+        <v>#DIV/0!</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A34" s="4"/>
-      <c r="B34" s="4"/>
-      <c r="C34" s="5">
-        <f>B34/(C2*37000)</f>
-        <v>0</v>
+      <c r="A34" s="3"/>
+      <c r="B34" s="3"/>
+      <c r="C34" s="4" t="e">
+        <f>B34/(E2*37000)</f>
+        <v>#DIV/0!</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A35" s="4"/>
-      <c r="B35" s="4"/>
-      <c r="C35" s="5">
-        <f>B35/(C2*37000)</f>
-        <v>0</v>
+      <c r="A35" s="3"/>
+      <c r="B35" s="3"/>
+      <c r="C35" s="4" t="e">
+        <f>B35/(E2*37000)</f>
+        <v>#DIV/0!</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A36" s="4"/>
-      <c r="B36" s="4"/>
-      <c r="C36" s="5">
-        <f>B36/(C2*37000)</f>
-        <v>0</v>
+      <c r="A36" s="3"/>
+      <c r="B36" s="3"/>
+      <c r="C36" s="4" t="e">
+        <f>B36/(E2*37000)</f>
+        <v>#DIV/0!</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A37" s="4"/>
-      <c r="B37" s="4"/>
-      <c r="C37" s="5">
-        <f>B37/(C2*37000)</f>
-        <v>0</v>
+      <c r="A37" s="3"/>
+      <c r="B37" s="3"/>
+      <c r="C37" s="4" t="e">
+        <f>B37/(E2*37000)</f>
+        <v>#DIV/0!</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A38" s="4"/>
-      <c r="B38" s="4"/>
-      <c r="C38" s="5">
-        <f>B38/(C2*37000)</f>
-        <v>0</v>
+      <c r="A38" s="3"/>
+      <c r="B38" s="3"/>
+      <c r="C38" s="4" t="e">
+        <f>B38/(E2*37000)</f>
+        <v>#DIV/0!</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A39" s="4"/>
-      <c r="B39" s="4"/>
-      <c r="C39" s="5">
-        <f>B39/(C2*37000)</f>
-        <v>0</v>
+      <c r="A39" s="3"/>
+      <c r="B39" s="3"/>
+      <c r="C39" s="4" t="e">
+        <f>B39/(E2*37000)</f>
+        <v>#DIV/0!</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A40" s="4"/>
-      <c r="B40" s="4"/>
-      <c r="C40" s="5">
-        <f>B40/(C2*37000)</f>
-        <v>0</v>
+      <c r="A40" s="3"/>
+      <c r="B40" s="3"/>
+      <c r="C40" s="4" t="e">
+        <f>B40/(E2*37000)</f>
+        <v>#DIV/0!</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A41" s="4"/>
-      <c r="B41" s="4"/>
-      <c r="C41" s="5">
-        <f>B41/(C2*37000)</f>
-        <v>0</v>
+      <c r="A41" s="3"/>
+      <c r="B41" s="3"/>
+      <c r="C41" s="4" t="e">
+        <f>B41/(E2*37000)</f>
+        <v>#DIV/0!</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A42" s="4"/>
-      <c r="B42" s="4"/>
-      <c r="C42" s="5">
-        <f>B42/(C2*37000)</f>
-        <v>0</v>
+      <c r="A42" s="3"/>
+      <c r="B42" s="3"/>
+      <c r="C42" s="4" t="e">
+        <f>B42/(E2*37000)</f>
+        <v>#DIV/0!</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A43" s="4"/>
-      <c r="B43" s="4"/>
-      <c r="C43" s="5">
-        <f>B43/(C2*37000)</f>
-        <v>0</v>
+      <c r="A43" s="3"/>
+      <c r="B43" s="3"/>
+      <c r="C43" s="4" t="e">
+        <f>B43/(E2*37000)</f>
+        <v>#DIV/0!</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A44" s="4"/>
-      <c r="B44" s="4"/>
-      <c r="C44" s="5">
-        <f>B44/(C2*37000)</f>
-        <v>0</v>
+      <c r="A44" s="3"/>
+      <c r="B44" s="3"/>
+      <c r="C44" s="4" t="e">
+        <f>B44/(E2*37000)</f>
+        <v>#DIV/0!</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A45" s="4"/>
-      <c r="B45" s="4"/>
-      <c r="C45" s="5">
-        <f>B45/(C2*37000)</f>
-        <v>0</v>
+      <c r="A45" s="3"/>
+      <c r="B45" s="3"/>
+      <c r="C45" s="4" t="e">
+        <f>B45/(E2*37000)</f>
+        <v>#DIV/0!</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A46" s="4"/>
-      <c r="B46" s="4"/>
-      <c r="C46" s="5">
-        <f>B46/(C2*37000)</f>
-        <v>0</v>
+      <c r="A46" s="3"/>
+      <c r="B46" s="3"/>
+      <c r="C46" s="4" t="e">
+        <f>B46/(E2*37000)</f>
+        <v>#DIV/0!</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A47" s="4"/>
-      <c r="B47" s="4"/>
-      <c r="C47" s="5">
-        <f>B47/(C2*37000)</f>
-        <v>0</v>
+      <c r="A47" s="3"/>
+      <c r="B47" s="3"/>
+      <c r="C47" s="4" t="e">
+        <f>B47/(E2*37000)</f>
+        <v>#DIV/0!</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A48" s="4"/>
-      <c r="B48" s="4"/>
-      <c r="C48" s="5">
-        <f>B48/(C2*37000)</f>
-        <v>0</v>
+      <c r="A48" s="3"/>
+      <c r="B48" s="3"/>
+      <c r="C48" s="4" t="e">
+        <f>B48/(E2*37000)</f>
+        <v>#DIV/0!</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A49" s="4"/>
-      <c r="B49" s="4"/>
-      <c r="C49" s="5">
-        <f>B49/(C2*37000)</f>
-        <v>0</v>
+      <c r="A49" s="3"/>
+      <c r="B49" s="3"/>
+      <c r="C49" s="4" t="e">
+        <f>B49/(E2*37000)</f>
+        <v>#DIV/0!</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A50" s="4"/>
-      <c r="B50" s="4"/>
-      <c r="C50" s="5">
-        <f>B50/(C2*37000)</f>
-        <v>0</v>
+      <c r="A50" s="3"/>
+      <c r="B50" s="3"/>
+      <c r="C50" s="4" t="e">
+        <f>B50/(E2*37000)</f>
+        <v>#DIV/0!</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A51" s="4"/>
-      <c r="B51" s="4"/>
-      <c r="C51" s="5">
-        <f>B51/(C2*37000)</f>
-        <v>0</v>
+      <c r="A51" s="3"/>
+      <c r="B51" s="3"/>
+      <c r="C51" s="4" t="e">
+        <f>B51/(E2*37000)</f>
+        <v>#DIV/0!</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A52" s="4"/>
-      <c r="B52" s="4"/>
-      <c r="C52" s="5">
-        <f>B52/(C2*37000)</f>
-        <v>0</v>
+      <c r="A52" s="3"/>
+      <c r="B52" s="3"/>
+      <c r="C52" s="4" t="e">
+        <f>B52/(E2*37000)</f>
+        <v>#DIV/0!</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A53" s="4"/>
-      <c r="B53" s="4"/>
-      <c r="C53" s="5">
-        <f>B53/(C2*37000)</f>
-        <v>0</v>
+      <c r="A53" s="3"/>
+      <c r="B53" s="3"/>
+      <c r="C53" s="4" t="e">
+        <f>B53/(E2*37000)</f>
+        <v>#DIV/0!</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A54" s="4"/>
-      <c r="B54" s="4"/>
-      <c r="C54" s="5">
-        <f>B54/(C2*37000)</f>
-        <v>0</v>
+      <c r="A54" s="3"/>
+      <c r="B54" s="3"/>
+      <c r="C54" s="4" t="e">
+        <f>B54/(E2*37000)</f>
+        <v>#DIV/0!</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A55" s="4"/>
-      <c r="B55" s="4"/>
-      <c r="C55" s="5">
-        <f>B55/(C2*37000)</f>
-        <v>0</v>
+      <c r="A55" s="3"/>
+      <c r="B55" s="3"/>
+      <c r="C55" s="4" t="e">
+        <f>B55/(E2*37000)</f>
+        <v>#DIV/0!</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A56" s="4"/>
-      <c r="B56" s="4"/>
-      <c r="C56" s="5">
-        <f>B56/(C2*37000)</f>
-        <v>0</v>
+      <c r="A56" s="3"/>
+      <c r="B56" s="3"/>
+      <c r="C56" s="4" t="e">
+        <f>B56/(E2*37000)</f>
+        <v>#DIV/0!</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A57" s="4"/>
-      <c r="B57" s="4"/>
-      <c r="C57" s="5">
-        <f>B57/(C2*37000)</f>
-        <v>0</v>
+      <c r="A57" s="3"/>
+      <c r="B57" s="3"/>
+      <c r="C57" s="4" t="e">
+        <f>B57/(E2*37000)</f>
+        <v>#DIV/0!</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A58" s="4"/>
-      <c r="B58" s="4"/>
-      <c r="C58" s="5">
-        <f>B58/(C2*37000)</f>
-        <v>0</v>
+      <c r="A58" s="3"/>
+      <c r="B58" s="3"/>
+      <c r="C58" s="4" t="e">
+        <f>B58/(E2*37000)</f>
+        <v>#DIV/0!</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A59" s="4"/>
-      <c r="B59" s="4"/>
-      <c r="C59" s="5">
-        <f>B59/(C2*37000)</f>
-        <v>0</v>
+      <c r="A59" s="3"/>
+      <c r="B59" s="3"/>
+      <c r="C59" s="4" t="e">
+        <f>B59/(E2*37000)</f>
+        <v>#DIV/0!</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A60" s="4"/>
-      <c r="B60" s="4"/>
-      <c r="C60" s="5">
-        <f>B60/(C2*37000)</f>
-        <v>0</v>
+      <c r="A60" s="3"/>
+      <c r="B60" s="3"/>
+      <c r="C60" s="4" t="e">
+        <f>B60/(E2*37000)</f>
+        <v>#DIV/0!</v>
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A61" s="4"/>
-      <c r="B61" s="4"/>
-      <c r="C61" s="5">
-        <f>B61/(C2*37000)</f>
-        <v>0</v>
+      <c r="A61" s="3"/>
+      <c r="B61" s="3"/>
+      <c r="C61" s="4" t="e">
+        <f>B61/(E2*37000)</f>
+        <v>#DIV/0!</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A62" s="4"/>
-      <c r="B62" s="4"/>
-      <c r="C62" s="5">
-        <f>B62/(C2*37000)</f>
-        <v>0</v>
+      <c r="A62" s="3"/>
+      <c r="B62" s="3"/>
+      <c r="C62" s="4" t="e">
+        <f>B62/(E2*37000)</f>
+        <v>#DIV/0!</v>
       </c>
     </row>
   </sheetData>

</xml_diff>